<commit_message>
Can now import Employees and Assets into SQL
Checks to see if item in .xlsx table exists, if it does then it isn't added to the database and displays a console notification that states the item that already exists.

We should add some GUI notifications for whether the import was successful or not and maybe save what those items were in a .xlsx file or something
</commit_message>
<xml_diff>
--- a/employeeList.xlsx
+++ b/employeeList.xlsx
@@ -1,11 +1,11 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="20730"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="23628"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2F5F310E-1338-47FF-8D70-3300135CB2FE}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{91E2B418-48AF-4129-A8F1-5F2ABC95CF67}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12645" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="390" yWindow="390" windowWidth="21600" windowHeight="11385" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="9" uniqueCount="9">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="10" uniqueCount="10">
   <si>
     <t>Name</t>
   </si>
@@ -47,6 +47,9 @@
   </si>
   <si>
     <t>Macha</t>
+  </si>
+  <si>
+    <t>Blazit</t>
   </si>
 </sst>
 </file>
@@ -82,8 +85,9 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -364,76 +368,84 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:B8"/>
+  <dimension ref="A1:B9"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D13" sqref="D13"/>
+      <selection activeCell="A9" sqref="A9:XFD9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A1" t="s">
+      <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="B1" t="s">
+      <c r="B1" s="1" t="s">
         <v>1</v>
       </c>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A2" t="s">
+      <c r="A2" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="B2">
+      <c r="B2" s="1">
         <v>3453123</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A3" t="s">
+      <c r="A3" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="B3">
+      <c r="B3" s="1">
         <v>543513</v>
       </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A4" t="s">
+      <c r="A4" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="B4">
+      <c r="B4" s="1">
         <v>12315315</v>
       </c>
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A5" t="s">
+      <c r="A5" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="B5">
+      <c r="B5" s="1">
         <v>153153</v>
       </c>
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A6" t="s">
+      <c r="A6" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="B6">
+      <c r="B6" s="1">
         <v>21313</v>
       </c>
     </row>
     <row r="7" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A7" t="s">
+      <c r="A7" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="B7">
+      <c r="B7" s="1">
         <v>1534753</v>
       </c>
     </row>
     <row r="8" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A8" t="s">
+      <c r="A8" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="B8">
+      <c r="B8" s="1">
         <v>123135</v>
+      </c>
+    </row>
+    <row r="9" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A9" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="B9">
+        <v>420420</v>
       </c>
     </row>
   </sheetData>

</xml_diff>